<commit_message>
adding the excel of methodlogies
</commit_message>
<xml_diff>
--- a/data/Attrakdiff.xlsx
+++ b/data/Attrakdiff.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/8-Enseñanza/RR-workshop/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175AE6E9-5610-C141-AF7F-666E92C99E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF16701-5973-9348-BF99-BCDB9E5F29EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="22020" windowHeight="15600" xr2:uid="{E38497EA-B483-2C43-9968-36BF0C541ADF}"/>
+    <workbookView xWindow="11580" yWindow="5400" windowWidth="22020" windowHeight="15600" activeTab="1" xr2:uid="{E38497EA-B483-2C43-9968-36BF0C541ADF}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="UEQ" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,9 +35,194 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="60">
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Agaçant</t>
+  </si>
+  <si>
+    <t>Agréable</t>
+  </si>
+  <si>
+    <t>Attraction</t>
+  </si>
+  <si>
+    <t>Incompréhensible</t>
+  </si>
+  <si>
+    <t>Compréhensible</t>
+  </si>
+  <si>
+    <t>Compréhensibilité</t>
+  </si>
+  <si>
+    <t>Moderne</t>
+  </si>
+  <si>
+    <t>Sans fantaisie</t>
+  </si>
+  <si>
+    <t>Originalité</t>
+  </si>
+  <si>
+    <t>Appropriation simple</t>
+  </si>
+  <si>
+    <t>Appropriation compliquée</t>
+  </si>
+  <si>
+    <t>Apporte de la valeur</t>
+  </si>
+  <si>
+    <t>Peu de valeur ajoutée</t>
+  </si>
+  <si>
+    <t>Stimulation</t>
+  </si>
+  <si>
+    <t>Ennuyeux</t>
+  </si>
+  <si>
+    <t>Captivant</t>
+  </si>
+  <si>
+    <t>Inintéressant</t>
+  </si>
+  <si>
+    <t>Intéressant</t>
+  </si>
+  <si>
+    <t>Imprévisible</t>
+  </si>
+  <si>
+    <t>Prévisible</t>
+  </si>
+  <si>
+    <t>Contrôlabilité</t>
+  </si>
+  <si>
+    <t>Rapide</t>
+  </si>
+  <si>
+    <t>Lent</t>
+  </si>
+  <si>
+    <t>Efficacité</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Conventionnel</t>
+  </si>
+  <si>
+    <t>Rigide</t>
+  </si>
+  <si>
+    <t>Facilitant</t>
+  </si>
+  <si>
+    <t>Bien</t>
+  </si>
+  <si>
+    <t>Médiocre</t>
+  </si>
+  <si>
+    <t>Compliqué</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Repoussant</t>
+  </si>
+  <si>
+    <t>Attractif</t>
+  </si>
+  <si>
+    <t>Habituel</t>
+  </si>
+  <si>
+    <t>Avant-gardiste</t>
+  </si>
+  <si>
+    <t>Désagréable</t>
+  </si>
+  <si>
+    <t>Sécurisant</t>
+  </si>
+  <si>
+    <t>Insécurisant</t>
+  </si>
+  <si>
+    <t>Stimulant</t>
+  </si>
+  <si>
+    <t>Soporifique</t>
+  </si>
+  <si>
+    <t>Répond aux attentes</t>
+  </si>
+  <si>
+    <t>Ne répond pas aux attentes</t>
+  </si>
+  <si>
+    <t>Inefficace</t>
+  </si>
+  <si>
+    <t>Efficace</t>
+  </si>
+  <si>
+    <t>Clair</t>
+  </si>
+  <si>
+    <t>Déroutant</t>
+  </si>
+  <si>
+    <t>Non pragmatique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pragmatique </t>
+  </si>
+  <si>
+    <t>Sobre</t>
+  </si>
+  <si>
+    <t>Surchargé</t>
+  </si>
+  <si>
+    <t>Attrayant</t>
+  </si>
+  <si>
+    <t>Rébarbatif</t>
+  </si>
+  <si>
+    <t>Sympathique</t>
+  </si>
+  <si>
+    <t>Inamical</t>
+  </si>
+  <si>
+    <t>Conservateur</t>
+  </si>
+  <si>
+    <t>Innovant</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,16 +230,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -61,12 +265,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,10 +656,327 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0EBBD9A-C5D2-7C48-BC50-9180C6A3C69B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AD8D8D-D8C9-8948-9853-BC0A218B380F}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>